<commit_message>
add Time Variant Request
</commit_message>
<xml_diff>
--- a/data/Scenario.xlsx
+++ b/data/Scenario.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20367"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B5D8E5-F37F-4A17-AB2C-A0B345D5F2BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ABF9F43-D88C-4F3D-A160-83B9771E5ADD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3196,15 +3196,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
+      <xdr:colOff>333375</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>41922</xdr:colOff>
+      <xdr:colOff>89547</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>131454</xdr:rowOff>
+      <xdr:rowOff>83829</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3233,7 +3233,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4581525" y="3143250"/>
+          <a:off x="4629150" y="3095625"/>
           <a:ext cx="5852172" cy="4389129"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3287,15 +3287,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
+      <xdr:colOff>352425</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>222897</xdr:colOff>
+      <xdr:colOff>108597</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>150504</xdr:rowOff>
+      <xdr:rowOff>179079</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3324,7 +3324,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4762500" y="3162300"/>
+          <a:off x="4648200" y="3190875"/>
           <a:ext cx="5852172" cy="4389129"/>
         </a:xfrm>
         <a:prstGeom prst="rect">

</xml_diff>

<commit_message>
modify System power consumption
</commit_message>
<xml_diff>
--- a/data/Scenario.xlsx
+++ b/data/Scenario.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20367"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20368"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8373350-9851-49EE-8986-A4678DEA5C6A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E752A96-9100-4965-9945-E1F6851CABC6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Benchmark" sheetId="1" r:id="rId1"/>
     <sheet name="Topology" sheetId="2" r:id="rId2"/>
-    <sheet name="10.4.L.5.2" sheetId="6" r:id="rId3"/>
-    <sheet name="40.10.L.5.2" sheetId="4" r:id="rId4"/>
+    <sheet name="PK" sheetId="7" r:id="rId3"/>
+    <sheet name="10.4.L.5.2" sheetId="6" r:id="rId4"/>
+    <sheet name="40.10.L.5.2" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="48">
   <si>
     <t>Benckmark4</t>
   </si>
@@ -178,6 +179,43 @@
     <t>Change/30 Itr</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>不知道preferrence vector</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>知道preferrence vector</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不須決定最大連線數</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>需要依照L計算</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>以最大EE為目標</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>只有caching是最小化Hit Rate來最小P_sys，間接最小化EE
+畫出所有L，找一個最好的EE跟RL PK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>可以嘗試SINR Benchmark</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">坤霖: Req的itr變大, 簡老師: Req先不變, implement time variant channel </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Benchmark(知道越多越好)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -287,13 +325,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -4053,10 +4091,10 @@
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="4"/>
+      <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -4137,7 +4175,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF2986BB-8F33-4471-B2CE-FA432FAA1E32}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
@@ -4212,7 +4250,7 @@
       <c r="G2" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="3" t="s">
         <v>21</v>
       </c>
       <c r="I2" s="2" t="s">
@@ -4317,7 +4355,7 @@
       <c r="G5" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="3" t="s">
         <v>38</v>
       </c>
       <c r="I5" s="2" t="s">
@@ -4394,10 +4432,73 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FEF6104-0AEE-4F14-8857-912AAFD3EEC7}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FDA256B-DC29-4143-B768-1CA233B3CDB4}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B35" sqref="B34:B35"/>
     </sheetView>
   </sheetViews>
@@ -4569,11 +4670,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A3AD492-D7C7-4493-A452-D08A68A80FDE}">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
new Time Variant Channel
</commit_message>
<xml_diff>
--- a/data/Scenario.xlsx
+++ b/data/Scenario.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20368"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33FDE2E2-0927-4494-83C6-4249DC115955}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96725C9E-2228-4841-9C30-44F1240FF8B4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -833,6 +833,7 @@
       <c:valAx>
         <c:axId val="997902272"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1976,6 +1977,7 @@
       <c:valAx>
         <c:axId val="994098960"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -3533,15 +3535,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>433387</xdr:colOff>
+      <xdr:colOff>119062</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>128587</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>423862</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3674,15 +3676,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:colOff>47625</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:rowOff>147637</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
+      <xdr:colOff>352425</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:rowOff>90487</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4406,7 +4408,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4584,7 +4586,7 @@
   <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D41"/>
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>